<commit_message>
Updates for class submission
Includes some bug fixes from end to end testing, and a final redaction
of the form to be as similar to the GBE site as a first pass would get
us.
</commit_message>
<xml_diff>
--- a/Priv and Nav.xlsx
+++ b/Priv and Nav.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="0" windowWidth="25600" windowHeight="15740" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="0" windowWidth="25600" windowHeight="15740" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="INTERCODE" sheetId="1" r:id="rId1"/>
     <sheet name="GBE" sheetId="2" r:id="rId2"/>
     <sheet name="Whos Who" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -103,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="181">
   <si>
     <t>Intercon Schedule navigation</t>
   </si>
@@ -619,6 +620,33 @@
   </si>
   <si>
     <t>PRIV_ADMIN</t>
+  </si>
+  <si>
+    <t>Bids.ph</t>
+  </si>
+  <si>
+    <t>is riddled through the code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bid Chair, GM Liason, the submitter, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is a function can_edit_game_info </t>
+  </si>
+  <si>
+    <t xml:space="preserve">change bid status </t>
+  </si>
+  <si>
+    <t>Bid Com, Bid Chair, GM Liason</t>
+  </si>
+  <si>
+    <t>Can all view bid committee feedback</t>
+  </si>
+  <si>
+    <t>bid chair</t>
+  </si>
+  <si>
+    <t>can update committee response</t>
   </si>
 </sst>
 </file>
@@ -930,12 +958,6 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -961,6 +983,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="111">
@@ -1405,11 +1433,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8420" ySplit="2240" topLeftCell="E10" activePane="bottomRight"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="8420" ySplit="2240" topLeftCell="E26" activePane="bottomLeft"/>
       <selection activeCell="I3" sqref="I3"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
       <selection pane="topRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34:XFD34"/>
       <selection pane="bottomRight" activeCell="E37" sqref="E37:F37"/>
     </sheetView>
   </sheetViews>
@@ -1433,23 +1461,23 @@
       <c r="A2" t="s">
         <v>146</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="21" t="s">
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="T2" s="21"/>
+      <c r="T2" s="31"/>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" ht="54">
       <c r="A3" s="1" t="s">
@@ -1476,7 +1504,7 @@
       <c r="H3" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="28" t="s">
         <v>162</v>
       </c>
       <c r="J3" s="16" t="s">
@@ -1485,7 +1513,7 @@
       <c r="K3" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="24" t="s">
         <v>164</v>
       </c>
       <c r="M3" s="16" t="s">
@@ -1494,13 +1522,13 @@
       <c r="N3" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="O3" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="Q3" s="30" t="s">
+      <c r="Q3" s="28" t="s">
         <v>167</v>
       </c>
       <c r="R3" s="16" t="s">
@@ -1509,7 +1537,7 @@
       <c r="S3" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="T3" s="31" t="s">
+      <c r="T3" s="29" t="s">
         <v>171</v>
       </c>
     </row>
@@ -1753,13 +1781,13 @@
       <c r="D8" t="s">
         <v>104</v>
       </c>
-      <c r="G8" s="25" t="str">
+      <c r="G8" s="23" t="str">
         <f t="shared" si="0"/>
         <v>Edit My Bio</v>
       </c>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
-      <c r="J8" s="25" t="str">
+      <c r="J8" s="23" t="str">
         <f t="shared" si="0"/>
         <v>Edit My Bio</v>
       </c>
@@ -3281,52 +3309,52 @@
       <c r="C39" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E39" s="27" t="s">
+      <c r="E39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F39" s="27" t="s">
+      <c r="F39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="G39" s="27" t="s">
+      <c r="G39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="H39" s="27" t="s">
+      <c r="H39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="I39" s="27" t="s">
+      <c r="I39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="J39" s="27" t="s">
+      <c r="J39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="K39" s="27" t="s">
+      <c r="K39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="L39" s="27" t="s">
+      <c r="L39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="M39" s="27" t="s">
+      <c r="M39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="N39" s="27" t="s">
+      <c r="N39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="O39" s="27" t="s">
+      <c r="O39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="P39" s="27" t="s">
+      <c r="P39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="Q39" s="27" t="s">
+      <c r="Q39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="R39" s="27" t="s">
+      <c r="R39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="S39" s="27" t="s">
+      <c r="S39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="T39" s="27" t="s">
+      <c r="T39" s="25" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3340,52 +3368,52 @@
       <c r="D40" t="s">
         <v>87</v>
       </c>
-      <c r="E40" s="28" t="s">
+      <c r="E40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F40" s="28" t="s">
+      <c r="F40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="G40" s="28" t="s">
+      <c r="G40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="H40" s="28" t="s">
+      <c r="H40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="I40" s="28" t="s">
+      <c r="I40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="J40" s="28" t="s">
+      <c r="J40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="K40" s="28" t="s">
+      <c r="K40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="L40" s="28" t="s">
+      <c r="L40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="M40" s="28" t="s">
+      <c r="M40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="N40" s="28" t="s">
+      <c r="N40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O40" s="28" t="s">
+      <c r="O40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="P40" s="28" t="s">
+      <c r="P40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="Q40" s="28" t="s">
+      <c r="Q40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="R40" s="28" t="s">
+      <c r="R40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="S40" s="28" t="s">
+      <c r="S40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="T40" s="28" t="s">
+      <c r="T40" s="26" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3505,7 +3533,7 @@
       <c r="J47" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M47" s="29" t="s">
+      <c r="M47" s="27" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4168,63 +4196,63 @@
       <c r="D89" t="s">
         <v>157</v>
       </c>
-      <c r="E89" s="22" t="str">
+      <c r="E89" s="20" t="str">
         <f t="shared" si="5"/>
         <v>preset able links hardcoded</v>
       </c>
-      <c r="F89" s="22" t="str">
+      <c r="F89" s="20" t="str">
         <f t="shared" si="5"/>
         <v>preset able links hardcoded</v>
       </c>
-      <c r="G89" s="22" t="str">
+      <c r="G89" s="20" t="str">
         <f t="shared" si="5"/>
         <v>preset able links hardcoded</v>
       </c>
-      <c r="H89" s="22" t="str">
+      <c r="H89" s="20" t="str">
         <f t="shared" si="5"/>
         <v>preset able links hardcoded</v>
       </c>
-      <c r="I89" s="22" t="str">
+      <c r="I89" s="20" t="str">
         <f t="shared" si="5"/>
         <v>preset able links hardcoded</v>
       </c>
-      <c r="J89" s="22" t="str">
+      <c r="J89" s="20" t="str">
         <f t="shared" si="5"/>
         <v>preset able links hardcoded</v>
       </c>
-      <c r="K89" s="22" t="str">
+      <c r="K89" s="20" t="str">
         <f t="shared" si="5"/>
         <v>preset able links hardcoded</v>
       </c>
-      <c r="L89" s="22" t="str">
+      <c r="L89" s="20" t="str">
         <f t="shared" si="5"/>
         <v>preset able links hardcoded</v>
       </c>
-      <c r="M89" s="22" t="str">
+      <c r="M89" s="20" t="str">
         <f t="shared" si="5"/>
         <v>preset able links hardcoded</v>
       </c>
-      <c r="N89" s="22" t="str">
+      <c r="N89" s="20" t="str">
         <f t="shared" si="5"/>
         <v>preset able links hardcoded</v>
       </c>
-      <c r="O89" s="22" t="str">
+      <c r="O89" s="20" t="str">
         <f t="shared" si="5"/>
         <v>preset able links hardcoded</v>
       </c>
-      <c r="P89" s="22" t="str">
+      <c r="P89" s="20" t="str">
         <f t="shared" si="5"/>
         <v>preset able links hardcoded</v>
       </c>
-      <c r="Q89" s="22" t="str">
+      <c r="Q89" s="20" t="str">
         <f t="shared" si="5"/>
         <v>preset able links hardcoded</v>
       </c>
-      <c r="R89" s="22" t="str">
+      <c r="R89" s="20" t="str">
         <f t="shared" si="5"/>
         <v>preset able links hardcoded</v>
       </c>
-      <c r="S89" s="23" t="s">
+      <c r="S89" s="21" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4235,63 +4263,63 @@
       <c r="C90" t="s">
         <v>151</v>
       </c>
-      <c r="E90" s="22" t="str">
+      <c r="E90" s="20" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">Community links </v>
       </c>
-      <c r="F90" s="22" t="str">
+      <c r="F90" s="20" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">Community links </v>
       </c>
-      <c r="G90" s="22" t="str">
+      <c r="G90" s="20" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">Community links </v>
       </c>
-      <c r="H90" s="22" t="str">
+      <c r="H90" s="20" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">Community links </v>
       </c>
-      <c r="I90" s="22" t="str">
+      <c r="I90" s="20" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">Community links </v>
       </c>
-      <c r="J90" s="22" t="str">
+      <c r="J90" s="20" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">Community links </v>
       </c>
-      <c r="K90" s="22" t="str">
+      <c r="K90" s="20" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">Community links </v>
       </c>
-      <c r="L90" s="22" t="str">
+      <c r="L90" s="20" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">Community links </v>
       </c>
-      <c r="M90" s="22" t="str">
+      <c r="M90" s="20" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">Community links </v>
       </c>
-      <c r="N90" s="22" t="str">
+      <c r="N90" s="20" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">Community links </v>
       </c>
-      <c r="O90" s="22" t="str">
+      <c r="O90" s="20" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">Community links </v>
       </c>
-      <c r="P90" s="22" t="str">
+      <c r="P90" s="20" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">Community links </v>
       </c>
-      <c r="Q90" s="22" t="str">
+      <c r="Q90" s="20" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">Community links </v>
       </c>
-      <c r="R90" s="22" t="str">
+      <c r="R90" s="20" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">Community links </v>
       </c>
-      <c r="S90" s="23" t="s">
+      <c r="S90" s="21" t="s">
         <v>154</v>
       </c>
     </row>
@@ -4305,63 +4333,63 @@
       <c r="D91" t="s">
         <v>158</v>
       </c>
-      <c r="E91" s="22" t="str">
+      <c r="E91" s="20" t="str">
         <f t="shared" si="5"/>
         <v>dynamic links made by staff</v>
       </c>
-      <c r="F91" s="22" t="str">
+      <c r="F91" s="20" t="str">
         <f t="shared" si="5"/>
         <v>dynamic links made by staff</v>
       </c>
-      <c r="G91" s="22" t="str">
+      <c r="G91" s="20" t="str">
         <f t="shared" si="5"/>
         <v>dynamic links made by staff</v>
       </c>
-      <c r="H91" s="22" t="str">
+      <c r="H91" s="20" t="str">
         <f t="shared" si="5"/>
         <v>dynamic links made by staff</v>
       </c>
-      <c r="I91" s="22" t="str">
+      <c r="I91" s="20" t="str">
         <f t="shared" si="5"/>
         <v>dynamic links made by staff</v>
       </c>
-      <c r="J91" s="22" t="str">
+      <c r="J91" s="20" t="str">
         <f t="shared" si="5"/>
         <v>dynamic links made by staff</v>
       </c>
-      <c r="K91" s="22" t="str">
+      <c r="K91" s="20" t="str">
         <f t="shared" si="5"/>
         <v>dynamic links made by staff</v>
       </c>
-      <c r="L91" s="22" t="str">
+      <c r="L91" s="20" t="str">
         <f t="shared" si="5"/>
         <v>dynamic links made by staff</v>
       </c>
-      <c r="M91" s="22" t="str">
+      <c r="M91" s="20" t="str">
         <f t="shared" si="5"/>
         <v>dynamic links made by staff</v>
       </c>
-      <c r="N91" s="22" t="str">
+      <c r="N91" s="20" t="str">
         <f t="shared" si="5"/>
         <v>dynamic links made by staff</v>
       </c>
-      <c r="O91" s="22" t="str">
+      <c r="O91" s="20" t="str">
         <f t="shared" si="5"/>
         <v>dynamic links made by staff</v>
       </c>
-      <c r="P91" s="22" t="str">
+      <c r="P91" s="20" t="str">
         <f t="shared" si="5"/>
         <v>dynamic links made by staff</v>
       </c>
-      <c r="Q91" s="22" t="str">
+      <c r="Q91" s="20" t="str">
         <f t="shared" si="5"/>
         <v>dynamic links made by staff</v>
       </c>
-      <c r="R91" s="22" t="str">
+      <c r="R91" s="20" t="str">
         <f t="shared" si="5"/>
         <v>dynamic links made by staff</v>
       </c>
-      <c r="S91" s="24" t="s">
+      <c r="S91" s="22" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4403,7 +4431,7 @@
   <dimension ref="A1:B92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5041,4 +5069,73 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Rehab in the events calendar
- removed excessive head counting
- 12 hour clock
- removed GM references
- separated Act/Bid some more
- fixed some bugs that happen when no one has a gender
</commit_message>
<xml_diff>
--- a/Priv and Nav.xlsx
+++ b/Priv and Nav.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="0" windowWidth="25600" windowHeight="15740" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="1040" yWindow="0" windowWidth="25600" windowHeight="15780" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="INTERCODE" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="184">
   <si>
     <t>Intercon Schedule navigation</t>
   </si>
@@ -647,6 +647,15 @@
   </si>
   <si>
     <t>can update committee response</t>
+  </si>
+  <si>
+    <t>$can_edit_game</t>
+  </si>
+  <si>
+    <t>Buried in Schedule - shows a whole new edit game link…</t>
+  </si>
+  <si>
+    <t>user_has_priv (PRIV_SCHEDULING) || user_has_priv (PRIV_GM_LIAISON)</t>
   </si>
 </sst>
 </file>
@@ -5073,10 +5082,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5130,6 +5139,19 @@
         <v>180</v>
       </c>
     </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" t="s">
+        <v>183</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>